<commit_message>
Revisions based on reviewer comments
Multiple changes based on reviewer comments
</commit_message>
<xml_diff>
--- a/data/Parallel/CombinedKinData_parallel.xlsx
+++ b/data/Parallel/CombinedKinData_parallel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anthony\Documents\GitHub\Lapsansky_Zatz_Tobalske_eLife_2020\data\Parallel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC095D15-F4E3-46A4-B1D1-BA558339A3D0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{110B5E54-0407-4FCA-94F5-BF2E546371EF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38655" yWindow="1140" windowWidth="14280" windowHeight="13710" xr2:uid="{150616B4-49CA-4136-994C-9CBCD5DEFFCD}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{150616B4-49CA-4136-994C-9CBCD5DEFFCD}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="38">
   <si>
     <t>Species</t>
   </si>
@@ -129,6 +129,24 @@
   </si>
   <si>
     <t>Downstroke Velocity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DownstrokeVelocity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UpstrokeVelocity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WingbeatFrequency </t>
+  </si>
+  <si>
+    <t>upduration</t>
+  </si>
+  <si>
+    <t>downduration</t>
+  </si>
+  <si>
+    <t>#ofWingbeats</t>
   </si>
 </sst>
 </file>
@@ -625,9 +643,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C14694BF-CA07-4D22-B41E-7CEC9E503429}">
   <dimension ref="A1:W81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N11" sqref="N11"/>
+      <selection pane="bottomLeft" activeCell="Q13" sqref="Q13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -656,22 +674,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="22" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="E1" s="22" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="G1" s="22" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="H1" s="22" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="I1" s="22" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -753,8 +771,9 @@
         <v>11</v>
       </c>
       <c r="K3" s="28"/>
-      <c r="L3" s="28"/>
-      <c r="M3" s="28"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
     </row>
     <row r="4" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A4" s="15" t="s">
@@ -787,8 +806,9 @@
         <v>11</v>
       </c>
       <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
     </row>
     <row r="5" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A5" s="15" t="s">
@@ -821,8 +841,9 @@
         <v>12</v>
       </c>
       <c r="K5" s="26"/>
-      <c r="L5" s="26"/>
-      <c r="M5" s="26"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
     </row>
     <row r="6" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A6" s="15" t="s">
@@ -855,8 +876,9 @@
         <v>12</v>
       </c>
       <c r="K6" s="26"/>
-      <c r="L6" s="26"/>
-      <c r="M6" s="26"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
     </row>
     <row r="7" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A7" s="15" t="s">
@@ -889,8 +911,9 @@
         <v>13</v>
       </c>
       <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
     </row>
     <row r="8" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A8" s="15" t="s">
@@ -923,8 +946,9 @@
         <v>11</v>
       </c>
       <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
     </row>
     <row r="9" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A9" s="15" t="s">
@@ -957,8 +981,9 @@
         <v>13</v>
       </c>
       <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
     </row>
     <row r="10" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A10" s="15" t="s">
@@ -991,8 +1016,9 @@
         <v>11</v>
       </c>
       <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
     </row>
     <row r="11" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A11" s="15" t="s">
@@ -1025,8 +1051,9 @@
         <v>10</v>
       </c>
       <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
     </row>
     <row r="12" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A12" s="11" t="s">
@@ -1057,8 +1084,9 @@
         <v>2.5</v>
       </c>
       <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
     </row>
     <row r="13" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A13" s="15" t="s">
@@ -1089,8 +1117,9 @@
         <v>4</v>
       </c>
       <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
     </row>
     <row r="14" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="15" t="s">
@@ -1121,8 +1150,9 @@
         <v>5</v>
       </c>
       <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
     </row>
     <row r="15" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A15" s="15" t="s">
@@ -1153,8 +1183,9 @@
         <v>7</v>
       </c>
       <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
     </row>
     <row r="16" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A16" s="15" t="s">
@@ -3136,7 +3167,7 @@
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>